<commit_message>
Update Verify from Excel
</commit_message>
<xml_diff>
--- a/Facebook_testingxlsx.xlsx
+++ b/Facebook_testingxlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\template_Works\robotframework_workshop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F058206-CF3E-4C65-8316-CC83BC95F328}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FBC934-DEA6-4F8E-BCB5-CCBE014720D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7020" yWindow="345" windowWidth="21600" windowHeight="11505" xr2:uid="{44FBDCB9-D13E-41AA-BE1E-CD9BF6680475}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>password</t>
   </si>
@@ -45,9 +45,6 @@
     <t>001</t>
   </si>
   <si>
-    <t>Thanawit.aki@gamail.com</t>
-  </si>
-  <si>
     <t>ธนาวิทย์ ชัยสุภาพสิริกุล</t>
   </si>
   <si>
@@ -57,10 +54,28 @@
     <t>002</t>
   </si>
   <si>
-    <t>"0831539901"</t>
-  </si>
-  <si>
     <t>u4704183</t>
+  </si>
+  <si>
+    <t>0831539901</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>nuthey@hotmail.com</t>
+  </si>
+  <si>
+    <t>Vasan247086;</t>
+  </si>
+  <si>
+    <t>Natty Nattha Tualek</t>
+  </si>
+  <si>
+    <t>Haleluyaa.aki@gamail.com</t>
+  </si>
+  <si>
+    <t>@Chai4704183;</t>
   </si>
 </sst>
 </file>
@@ -186,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -194,11 +209,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3656194-4893-4AF2-B64E-8B6E56D73EAD}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,53 +560,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="12"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="5">
-        <v>123456</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
+      <c r="B5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -602,6 +632,7 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{C67B55D6-BE34-4A0E-96DF-8501BBDCE4F5}"/>
     <hyperlink ref="B4" r:id="rId2" display="Thanawit.aki@gamail.com" xr:uid="{14A9B1E0-70DB-4AAB-824A-B092C8CAC52F}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{C54227F6-BE80-4433-8EB0-7A4018FC1EA5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>